<commit_message>
Added test project and a unit service for business logic
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Buck\source\repos\StudentRecords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA6A8195-4EE6-404C-BB3F-7351EF6D24D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47ECE8FA-7790-4A0B-B78F-ECEDB9BA880D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16688" windowHeight="7133" xr2:uid="{ACB52218-CABE-4B7C-95F4-8D3E75E53122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16688" windowHeight="7133" activeTab="1" xr2:uid="{ACB52218-CABE-4B7C-95F4-8D3E75E53122}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Home" sheetId="1" r:id="rId1"/>
+    <sheet name="Manage Units" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Scenario</t>
   </si>
@@ -106,6 +107,33 @@
   </si>
   <si>
     <t>The 'add results' form should be displayed that captures the unit code, student ID, student photo, semester number, year, assignment and/or exam</t>
+  </si>
+  <si>
+    <t>When a user adds a new unit</t>
+  </si>
+  <si>
+    <t>The new unit should be displayed in the Units table</t>
+  </si>
+  <si>
+    <t>When a user attempts to adds more than 7 alphanumeric characters to the unitcode</t>
+  </si>
+  <si>
+    <t>The text should not exceed 7 characters</t>
+  </si>
+  <si>
+    <t>When the user enters less than 7 characters in the unitcode</t>
+  </si>
+  <si>
+    <t>The user should be prompted to add 7 characters</t>
+  </si>
+  <si>
+    <t>When the user adds a unit title to a unit</t>
+  </si>
+  <si>
+    <t>The units table should reflect the unit with that unit title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the user </t>
   </si>
 </sst>
 </file>
@@ -462,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A656749A-3CE2-4ACD-96D9-7A26651B0607}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -505,7 +533,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="114" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -575,6 +603,69 @@
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F4C599-D41A-4A8A-989F-0AFA731F59A7}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="37.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="16384" width="37.73046875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>